<commit_message>
Modify khaosatPzem, co the lay data theo dia chi
</commit_message>
<xml_diff>
--- a/doc/khaoSatPzem004.xlsx
+++ b/doc/khaoSatPzem004.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
   <si>
     <t xml:space="preserve">f8 04 14 08 97 00 22 00 00 00 04 00 00 00 00 00 00 01 f5 00 05 00 00 a6 30                 ø...—."...........õ....¦0     </t>
   </si>
@@ -170,9 +170,6 @@
     <t>rep reset energy</t>
   </si>
   <si>
-    <t>Vao mode set parameter</t>
-  </si>
-  <si>
     <t>f8 03 00 00 00 07 10 61</t>
   </si>
   <si>
@@ -182,7 +179,31 @@
     <t>rep Vao mode set parameter</t>
   </si>
   <si>
-    <t>Add 1, AP 23000</t>
+    <t>f8 10 00 00 00 04 08 01 00 d8 59 2e 00 80 25 e9 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parameter - comand Read</t>
+  </si>
+  <si>
+    <t>set paramete</t>
+  </si>
+  <si>
+    <t>Add 46, AP 23000</t>
+  </si>
+  <si>
+    <t>f8 10 00 00 00 04 d5 a3</t>
+  </si>
+  <si>
+    <t>f8 10 00 00 00 04 08 01 00 d8 59 57 00 80 25 f0 4e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f8 10 00 00 00 04 d5 a3                                </t>
+  </si>
+  <si>
+    <t>2e 04 00 00 00 0a 77 92</t>
+  </si>
+  <si>
+    <t>dia chi 46</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1525,7 @@
     <col min="4" max="4" width="125.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1512,12 +1533,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -1525,7 +1546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>36</v>
       </c>
@@ -1541,7 +1562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1557,7 +1578,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1586,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -1573,7 +1594,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>36</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1610,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -1597,7 +1618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1605,12 +1626,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1631,23 +1660,42 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>